<commit_message>
Fixing bug when time is across multiple dates
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,269 +462,685 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3364</v>
+        <v>7366</v>
       </c>
       <c r="C2" t="n">
-        <v>406.57</v>
+        <v>958.8200000000002</v>
       </c>
       <c r="D2" t="n">
-        <v>496.4458764788351</v>
+        <v>460.9415740180638</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>rforootj</t>
+          <t>z</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6282</v>
+        <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>690.38</v>
+        <v>3.32</v>
       </c>
       <c r="D3" t="n">
-        <v>545.9601958341782</v>
+        <v>542.1686746987951</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RFOROOT</t>
+          <t>ashmom</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3837</v>
+        <v>1409</v>
       </c>
       <c r="C4" t="n">
-        <v>483.5</v>
+        <v>155.58</v>
       </c>
       <c r="D4" t="n">
-        <v>476.153050672182</v>
+        <v>543.3860393366757</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>rfosilvet</t>
+          <t>RFOCHAN</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6653</v>
+        <v>274</v>
       </c>
       <c r="C5" t="n">
-        <v>893.13</v>
+        <v>32.07</v>
       </c>
       <c r="D5" t="n">
-        <v>446.9450136038427</v>
+        <v>512.6286248830683</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>long</t>
+          <t>rfoaves</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>769</v>
+        <v>891</v>
       </c>
       <c r="C6" t="n">
-        <v>111.51</v>
+        <v>99.8</v>
       </c>
       <c r="D6" t="n">
-        <v>413.7745493677697</v>
+        <v>535.6713426853707</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>rfogatli</t>
+          <t>rfoschwa</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4346</v>
+        <v>1975</v>
       </c>
       <c r="C7" t="n">
-        <v>597.86</v>
+        <v>323.77</v>
       </c>
       <c r="D7" t="n">
-        <v>436.1556217174589</v>
+        <v>366.0005559502115</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>RFORoot</t>
+          <t>rfolindsj</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>91</v>
+        <v>2923</v>
       </c>
       <c r="C8" t="n">
-        <v>36.06</v>
+        <v>441.88</v>
       </c>
       <c r="D8" t="n">
-        <v>151.414309484193</v>
+        <v>396.8950846383634</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>rfoande</t>
+          <t>rfoalves</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>86</v>
+        <v>2563</v>
       </c>
       <c r="C9" t="n">
-        <v>29.64</v>
+        <v>281.02</v>
       </c>
       <c r="D9" t="n">
-        <v>174.0890688259109</v>
+        <v>547.2208383744929</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ashom</t>
+          <t>RFORoot</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="C10" t="n">
-        <v>13.92</v>
+        <v>36.06</v>
       </c>
       <c r="D10" t="n">
-        <v>250</v>
+        <v>151.414309484193</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>rfoander</t>
+          <t>RFOCARSOS</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4478</v>
+        <v>6537</v>
       </c>
       <c r="C11" t="n">
-        <v>629.05</v>
+        <v>877.55</v>
       </c>
       <c r="D11" t="n">
-        <v>427.1202607105954</v>
+        <v>446.948891801037</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RFOCARSOS</t>
+          <t>rfodel</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4749</v>
+        <v>7</v>
       </c>
       <c r="C12" t="n">
-        <v>670.3199999999999</v>
+        <v>0.22</v>
       </c>
       <c r="D12" t="n">
-        <v>425.0805585392052</v>
+        <v>1909.090909090909</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>.</t>
+          <t>RFODISCH</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1933</v>
+        <v>3743</v>
       </c>
       <c r="C13" t="n">
-        <v>188.63</v>
+        <v>538.17</v>
       </c>
       <c r="D13" t="n">
-        <v>614.8544770185018</v>
+        <v>417.3030826690451</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>RFOBROCK</t>
+          <t>rfosilvet</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3676</v>
+        <v>3033</v>
       </c>
       <c r="C14" t="n">
-        <v>443.73</v>
+        <v>281.51</v>
       </c>
       <c r="D14" t="n">
-        <v>497.0590223784734</v>
+        <v>646.4423999147455</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ashmom</t>
+          <t>RFOKSB162</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3858</v>
+        <v>2295</v>
       </c>
       <c r="C15" t="n">
-        <v>447.53</v>
+        <v>186.09</v>
       </c>
       <c r="D15" t="n">
-        <v>517.2390677719929</v>
+        <v>739.9645332903434</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>rfoghart</t>
+          <t>MAZZA</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4523</v>
+        <v>2110</v>
       </c>
       <c r="C16" t="n">
-        <v>567.66</v>
+        <v>190.27</v>
       </c>
       <c r="D16" t="n">
-        <v>478.0678575203466</v>
+        <v>665.3702633100331</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ashm</t>
+          <t>rfopiercn</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>90</v>
+        <v>1132</v>
       </c>
       <c r="C17" t="n">
-        <v>16.04</v>
+        <v>105.59</v>
       </c>
       <c r="D17" t="n">
-        <v>336.6583541147132</v>
+        <v>643.2427313192537</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>rfoksc071</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>3008</v>
+      </c>
+      <c r="C18" t="n">
+        <v>325.04</v>
+      </c>
+      <c r="D18" t="n">
+        <v>555.254737878415</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>rforootj</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2419</v>
+      </c>
+      <c r="C19" t="n">
+        <v>224.01</v>
+      </c>
+      <c r="D19" t="n">
+        <v>647.9175036828713</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>rfoghart</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1086</v>
+      </c>
+      <c r="C20" t="n">
+        <v>68.90000000000001</v>
+      </c>
+      <c r="D20" t="n">
+        <v>945.7184325108852</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>rfoksc905</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>582</v>
+      </c>
+      <c r="C21" t="n">
+        <v>59.72</v>
+      </c>
+      <c r="D21" t="n">
+        <v>584.7287340924314</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>RFOROOT</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1711</v>
+      </c>
+      <c r="C22" t="n">
+        <v>217.03</v>
+      </c>
+      <c r="D22" t="n">
+        <v>473.0221628346311</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>rfoander</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1763</v>
+      </c>
+      <c r="C23" t="n">
+        <v>201.78</v>
+      </c>
+      <c r="D23" t="n">
+        <v>524.2343146000595</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>RFOKSB167</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1853</v>
+      </c>
+      <c r="C24" t="n">
+        <v>186.01</v>
+      </c>
+      <c r="D24" t="n">
+        <v>597.7098005483576</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>rfoely</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>90</v>
+      </c>
+      <c r="C25" t="n">
+        <v>7.42</v>
+      </c>
+      <c r="D25" t="n">
+        <v>727.7628032345013</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>rfoalve</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1523</v>
+      </c>
+      <c r="C26" t="n">
+        <v>298.83</v>
+      </c>
+      <c r="D26" t="n">
+        <v>305.7925911053107</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>RFOBRADA</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2528</v>
+      </c>
+      <c r="C27" t="n">
+        <v>190.04</v>
+      </c>
+      <c r="D27" t="n">
+        <v>798.1477583666597</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>rfoksb170</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>440</v>
+      </c>
+      <c r="C28" t="n">
+        <v>58.35</v>
+      </c>
+      <c r="D28" t="n">
+        <v>452.4421593830334</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>rfalves</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>79</v>
+      </c>
+      <c r="C29" t="n">
+        <v>26.81</v>
+      </c>
+      <c r="D29" t="n">
+        <v>176.7997016038792</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>RFOKSB699</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1756</v>
+      </c>
+      <c r="C30" t="n">
+        <v>181.98</v>
+      </c>
+      <c r="D30" t="n">
+        <v>578.9647213979558</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>rfodeloy</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>7377</v>
+      </c>
+      <c r="C31" t="n">
+        <v>880.4299999999999</v>
+      </c>
+      <c r="D31" t="n">
+        <v>502.7316197767</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>RFOKSB164</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1707</v>
+      </c>
+      <c r="C32" t="n">
+        <v>188.7</v>
+      </c>
+      <c r="D32" t="n">
+        <v>542.7662957074722</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>RFOCLARK</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>5674</v>
-      </c>
-      <c r="C18" t="n">
-        <v>739.4100000000001</v>
-      </c>
-      <c r="D18" t="n">
-        <v>460.4211465898486</v>
+      <c r="B33" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C33" t="n">
+        <v>226.74</v>
+      </c>
+      <c r="D33" t="n">
+        <v>534.5329452236041</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>long</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1073</v>
+      </c>
+      <c r="C34" t="n">
+        <v>133.31</v>
+      </c>
+      <c r="D34" t="n">
+        <v>482.9345135398694</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>RFOKS171</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1900</v>
+      </c>
+      <c r="C35" t="n">
+        <v>188.24</v>
+      </c>
+      <c r="D35" t="n">
+        <v>605.6098597535062</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>mh</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>3993</v>
+      </c>
+      <c r="C36" t="n">
+        <v>483.08</v>
+      </c>
+      <c r="D36" t="n">
+        <v>495.9427010019044</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>RFOCOOK</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1729</v>
+      </c>
+      <c r="C37" t="n">
+        <v>191.31</v>
+      </c>
+      <c r="D37" t="n">
+        <v>542.2612513721185</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>RFOBROCK</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>7023</v>
+      </c>
+      <c r="C38" t="n">
+        <v>779.0399999999998</v>
+      </c>
+      <c r="D38" t="n">
+        <v>540.8964879852126</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1933</v>
+      </c>
+      <c r="C39" t="n">
+        <v>188.63</v>
+      </c>
+      <c r="D39" t="n">
+        <v>614.8544770185018</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>RFOKSB419</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>911</v>
+      </c>
+      <c r="C40" t="n">
+        <v>104.85</v>
+      </c>
+      <c r="D40" t="n">
+        <v>521.3161659513592</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>rfoksc041</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>7727</v>
+      </c>
+      <c r="C41" t="n">
+        <v>951.77</v>
+      </c>
+      <c r="D41" t="n">
+        <v>487.1134832995367</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>rfogatli</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>1291</v>
+      </c>
+      <c r="C42" t="n">
+        <v>113.89</v>
+      </c>
+      <c r="D42" t="n">
+        <v>680.1299499517077</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>RFOKSB183</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>182</v>
+      </c>
+      <c r="C43" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="D43" t="n">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>lee</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>81</v>
+      </c>
+      <c r="C44" t="n">
+        <v>5.63</v>
+      </c>
+      <c r="D44" t="n">
+        <v>863.2326820603907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>